<commit_message>
Ajout de listes déroulantes au dataset de validation 20 questions
## Modifications

**Fichier mis à jour :**
- output/validation_dataset_20questions.xlsx

**Nouvelles colonnes avec listes déroulantes :**
1. Type_Document (5 valeurs)
2. Domaine_Metier (3 valeurs : RH, DEONTOLOGIE, ASSURANCES)
3. Source_Document (8 sources techniques)
4. Thematiques (19 thématiques)
5. Mots_Cles (45 mots-clés)

**Nouveaux onglets de référence créés :**
- Ref_TypesDocument
- Ref_DomainesMetier
- Ref_SourcesDocument
- Ref_Thematiques
- Ref_MotsCles

**Script ajouté :**
- update_validation_dataset.py : script pour mettre à jour le fichier Excel

Toutes les valeurs des listes déroulantes sont extraites automatiquement
depuis l'index complet (_metadata/index_complet.json).

**Backup :**
- output/validation_dataset_20questions_backup.xlsx (version originale)
</commit_message>
<xml_diff>
--- a/output/validation_dataset_20questions.xlsx
+++ b/output/validation_dataset_20questions.xlsx
@@ -9,6 +9,11 @@
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Validation_Questions" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Ref_TypesDocument" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Ref_Thematiques" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Ref_MotsCles" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Ref_SourcesDocument" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Ref_DomainesMetier" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -501,7 +506,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -526,7 +530,6 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
@@ -534,7 +537,6 @@
         </is>
       </c>
     </row>
-    <row r="7"/>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
@@ -649,7 +651,6 @@
         </is>
       </c>
     </row>
-    <row r="20"/>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
@@ -671,7 +672,6 @@
         </is>
       </c>
     </row>
-    <row r="24"/>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
@@ -741,7 +741,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -786,67 +786,92 @@
           <t>Categorie</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Type_Document</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Domaine_Metier</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Source_Document</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Thematiques</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Mots_Cles</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>Difficulte</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>Documents_Sources_Proposes</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>Elements_Cles_Reponse</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>Reponse_Attendue_Resumee</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>Validation_Question</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>Correction_Question</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>Validation_Sources</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>Correction_Sources</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>Validation_Elements_Cles</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>Correction_Elements_Cles</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>Validation_Reponse_Attendue</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>Correction_Reponse_Attendue</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="U1" s="4" t="inlineStr">
         <is>
           <t>Commentaires</t>
         </is>
@@ -868,37 +893,37 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="I2" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t>csn2019_analyse_nationale_des_risques_lcb_ft_en_france_septembre_2019</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="K2" s="5" t="inlineStr">
         <is>
           <t>1. Lutte Contre le Blanchiment de capitaux
 2. Financement du Terrorisme
 3. Obligation légale pour les notaires</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="L2" s="5" t="inlineStr">
         <is>
           <t>LCB-FT signifie Lutte Contre le Blanchiment de capitaux et le Financement du Terrorisme. Il s'agit d'un ensemble d'obligations légales imposées aux notaires pour prévenir l'utilisation du système financier à des fins illégales.</t>
         </is>
       </c>
-      <c r="H2" s="6" t="n"/>
-      <c r="I2" s="5" t="n"/>
-      <c r="J2" s="6" t="n"/>
-      <c r="K2" s="5" t="n"/>
-      <c r="L2" s="6" t="n"/>
-      <c r="M2" s="5" t="n"/>
-      <c r="N2" s="7" t="n"/>
-      <c r="O2" s="7" t="n"/>
+      <c r="M2" s="6" t="n"/>
+      <c r="N2" s="5" t="n"/>
+      <c r="O2" s="6" t="n"/>
       <c r="P2" s="5" t="n"/>
+      <c r="Q2" s="6" t="n"/>
+      <c r="R2" s="5" t="n"/>
+      <c r="S2" s="7" t="n"/>
+      <c r="T2" s="7" t="n"/>
+      <c r="U2" s="5" t="n"/>
     </row>
     <row r="3" ht="60" customHeight="1">
       <c r="A3" s="5" t="inlineStr">
@@ -916,37 +941,37 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="I3" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="J3" s="5" t="inlineStr">
         <is>
           <t>rpn_rpn</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="K3" s="5" t="inlineStr">
         <is>
           <t>1. Règlement Professionnel du Notariat
 2. Entré en vigueur le 1er février 2024
 3. Approuvé par arrêté du Garde des Sceaux du 29 janvier 2024</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="L3" s="5" t="inlineStr">
         <is>
           <t>Le RPN est le Règlement Professionnel du Notariat. Il est entré en vigueur le 1er février 2024 après avoir été approuvé par arrêté du Garde des Sceaux en date du 29 janvier 2024. Il remplace l'ancien règlement national-règlement intercours.</t>
         </is>
       </c>
-      <c r="H3" s="6" t="n"/>
-      <c r="I3" s="5" t="n"/>
-      <c r="J3" s="6" t="n"/>
-      <c r="K3" s="5" t="n"/>
-      <c r="L3" s="6" t="n"/>
-      <c r="M3" s="5" t="n"/>
-      <c r="N3" s="7" t="n"/>
-      <c r="O3" s="7" t="n"/>
+      <c r="M3" s="6" t="n"/>
+      <c r="N3" s="5" t="n"/>
+      <c r="O3" s="6" t="n"/>
       <c r="P3" s="5" t="n"/>
+      <c r="Q3" s="6" t="n"/>
+      <c r="R3" s="5" t="n"/>
+      <c r="S3" s="7" t="n"/>
+      <c r="T3" s="7" t="n"/>
+      <c r="U3" s="5" t="n"/>
     </row>
     <row r="4" ht="60" customHeight="1">
       <c r="A4" s="5" t="inlineStr">
@@ -964,37 +989,37 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="I4" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="J4" s="5" t="inlineStr">
         <is>
           <t>rpn_rpn; fil_infos_fil_info_262</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="K4" s="5" t="inlineStr">
         <is>
           <t>1. 1er février 2024
 2. Décret du 28 décembre 2023
 3. En même temps que le RPN</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="L4" s="5" t="inlineStr">
         <is>
           <t>Le Code de déontologie des notaires est entré en vigueur le 1er février 2024, édicté par décret du 28 décembre 2023, en même temps que le Règlement Professionnel du Notariat (RPN).</t>
         </is>
       </c>
-      <c r="H4" s="6" t="n"/>
-      <c r="I4" s="5" t="n"/>
-      <c r="J4" s="6" t="n"/>
-      <c r="K4" s="5" t="n"/>
-      <c r="L4" s="6" t="n"/>
-      <c r="M4" s="5" t="n"/>
-      <c r="N4" s="7" t="n"/>
-      <c r="O4" s="7" t="n"/>
+      <c r="M4" s="6" t="n"/>
+      <c r="N4" s="5" t="n"/>
+      <c r="O4" s="6" t="n"/>
       <c r="P4" s="5" t="n"/>
+      <c r="Q4" s="6" t="n"/>
+      <c r="R4" s="5" t="n"/>
+      <c r="S4" s="7" t="n"/>
+      <c r="T4" s="7" t="n"/>
+      <c r="U4" s="5" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
       <c r="A5" s="5" t="inlineStr">
@@ -1012,37 +1037,37 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="I5" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="J5" s="5" t="inlineStr">
         <is>
           <t>fil_infos_fil_info_262</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="K5" s="5" t="inlineStr">
         <is>
           <t>1. Loi du 18 novembre 2021 pour la confiance dans l'institution judiciaire
 2. Ordonnance du 13 avril 2022
 3. Réforme profonde de la discipline et de la déontologie</t>
         </is>
       </c>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="L5" s="5" t="inlineStr">
         <is>
           <t>La loi du 18 novembre 2021 pour la confiance dans l'institution judiciaire et l'ordonnance du 13 avril 2022 ont réformé en profondeur la discipline et la déontologie notariale. Ces textes sont applicables à l'action des professionnels du droit, donc aux notaires.</t>
         </is>
       </c>
-      <c r="H5" s="6" t="n"/>
-      <c r="I5" s="5" t="n"/>
-      <c r="J5" s="6" t="n"/>
-      <c r="K5" s="5" t="n"/>
-      <c r="L5" s="6" t="n"/>
-      <c r="M5" s="5" t="n"/>
-      <c r="N5" s="7" t="n"/>
-      <c r="O5" s="7" t="n"/>
+      <c r="M5" s="6" t="n"/>
+      <c r="N5" s="5" t="n"/>
+      <c r="O5" s="6" t="n"/>
       <c r="P5" s="5" t="n"/>
+      <c r="Q5" s="6" t="n"/>
+      <c r="R5" s="5" t="n"/>
+      <c r="S5" s="7" t="n"/>
+      <c r="T5" s="7" t="n"/>
+      <c r="U5" s="5" t="n"/>
     </row>
     <row r="6" ht="60" customHeight="1">
       <c r="A6" s="5" t="inlineStr">
@@ -1060,17 +1085,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="I6" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
+      <c r="J6" s="5" t="inlineStr">
         <is>
           <t>csn2019_analyse_nationale_des_risques_lcb_ft_en_france_septembre_2019</t>
         </is>
       </c>
-      <c r="F6" s="5" t="inlineStr">
+      <c r="K6" s="5" t="inlineStr">
         <is>
           <t>1. Obligation devenue pratique professionnelle quotidienne
 2. Premiers contributeurs du secteur non-financier
@@ -1078,20 +1103,20 @@
 4. Prévenir le blanchiment de capitaux</t>
         </is>
       </c>
-      <c r="G6" s="5" t="inlineStr">
+      <c r="L6" s="5" t="inlineStr">
         <is>
           <t>Le notariat remplit un rôle important dans la LCB-FT qui est devenue une pratique professionnelle quotidienne. Les notaires sont les premiers contributeurs du secteur non-financier auprès du service de renseignement gouvernemental Tracfin, avec pour mission de prévenir l'utilisation du système financier à des fins de blanchiment.</t>
         </is>
       </c>
-      <c r="H6" s="6" t="n"/>
-      <c r="I6" s="5" t="n"/>
-      <c r="J6" s="6" t="n"/>
-      <c r="K6" s="5" t="n"/>
-      <c r="L6" s="6" t="n"/>
-      <c r="M6" s="5" t="n"/>
-      <c r="N6" s="7" t="n"/>
-      <c r="O6" s="7" t="n"/>
+      <c r="M6" s="6" t="n"/>
+      <c r="N6" s="5" t="n"/>
+      <c r="O6" s="6" t="n"/>
       <c r="P6" s="5" t="n"/>
+      <c r="Q6" s="6" t="n"/>
+      <c r="R6" s="5" t="n"/>
+      <c r="S6" s="7" t="n"/>
+      <c r="T6" s="7" t="n"/>
+      <c r="U6" s="5" t="n"/>
     </row>
     <row r="7" ht="60" customHeight="1">
       <c r="A7" s="5" t="inlineStr">
@@ -1109,17 +1134,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="E7" s="5" t="inlineStr">
+      <c r="J7" s="5" t="inlineStr">
         <is>
           <t>rpn_rpn</t>
         </is>
       </c>
-      <c r="F7" s="5" t="inlineStr">
+      <c r="K7" s="5" t="inlineStr">
         <is>
           <t>1. Acte reçu par un officier public (notaire)
 2. Confère foi publique à son contenu
@@ -1127,20 +1152,20 @@
 4. Force exécutoire</t>
         </is>
       </c>
-      <c r="G7" s="5" t="inlineStr">
+      <c r="L7" s="5" t="inlineStr">
         <is>
           <t>Un acte authentique est un acte reçu par un officier public, en l'occurrence le notaire, qui confère foi publique à son contenu. Il a une date certaine et possède une force exécutoire, ce qui lui donne une valeur juridique particulière.</t>
         </is>
       </c>
-      <c r="H7" s="6" t="n"/>
-      <c r="I7" s="5" t="n"/>
-      <c r="J7" s="6" t="n"/>
-      <c r="K7" s="5" t="n"/>
-      <c r="L7" s="6" t="n"/>
-      <c r="M7" s="5" t="n"/>
-      <c r="N7" s="7" t="n"/>
-      <c r="O7" s="7" t="n"/>
+      <c r="M7" s="6" t="n"/>
+      <c r="N7" s="5" t="n"/>
+      <c r="O7" s="6" t="n"/>
       <c r="P7" s="5" t="n"/>
+      <c r="Q7" s="6" t="n"/>
+      <c r="R7" s="5" t="n"/>
+      <c r="S7" s="7" t="n"/>
+      <c r="T7" s="7" t="n"/>
+      <c r="U7" s="5" t="n"/>
     </row>
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="5" t="inlineStr">
@@ -1158,17 +1183,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="D8" s="5" t="inlineStr">
+      <c r="I8" s="5" t="inlineStr">
         <is>
           <t>Pointu</t>
         </is>
       </c>
-      <c r="E8" s="5" t="inlineStr">
+      <c r="J8" s="5" t="inlineStr">
         <is>
           <t>rpn_rpn</t>
         </is>
       </c>
-      <c r="F8" s="5" t="inlineStr">
+      <c r="K8" s="5" t="inlineStr">
         <is>
           <t>1. Entrés en vigueur simultanément le 1er février 2024
 2. Code de déontologie édicté par décret en Conseil d'État
@@ -1178,20 +1203,20 @@
 6. Violation expose à des poursuites disciplinaires</t>
         </is>
       </c>
-      <c r="G8" s="5" t="inlineStr">
+      <c r="L8" s="5" t="inlineStr">
         <is>
           <t>Le Code de déontologie et le RPN sont deux textes complémentaires entrés en vigueur simultanément le 1er février 2024. Le Code de déontologie, édicté par décret en Conseil d'État, pose les principes déontologiques généraux. Le RPN, approuvé par arrêté du Garde des Sceaux, détaille les règles d'application pratiques. La violation de ces dispositions expose à des poursuites disciplinaires.</t>
         </is>
       </c>
-      <c r="H8" s="6" t="n"/>
-      <c r="I8" s="5" t="n"/>
-      <c r="J8" s="6" t="n"/>
-      <c r="K8" s="5" t="n"/>
-      <c r="L8" s="6" t="n"/>
-      <c r="M8" s="5" t="n"/>
-      <c r="N8" s="7" t="n"/>
-      <c r="O8" s="7" t="n"/>
+      <c r="M8" s="6" t="n"/>
+      <c r="N8" s="5" t="n"/>
+      <c r="O8" s="6" t="n"/>
       <c r="P8" s="5" t="n"/>
+      <c r="Q8" s="6" t="n"/>
+      <c r="R8" s="5" t="n"/>
+      <c r="S8" s="7" t="n"/>
+      <c r="T8" s="7" t="n"/>
+      <c r="U8" s="5" t="n"/>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="5" t="inlineStr">
@@ -1209,17 +1234,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="D9" s="5" t="inlineStr">
+      <c r="I9" s="5" t="inlineStr">
         <is>
           <t>Pointu</t>
         </is>
       </c>
-      <c r="E9" s="5" t="inlineStr">
+      <c r="J9" s="5" t="inlineStr">
         <is>
           <t>fil_infos_fil_info_265</t>
         </is>
       </c>
-      <c r="F9" s="5" t="inlineStr">
+      <c r="K9" s="5" t="inlineStr">
         <is>
           <t>1. Vision : société apaisée où les droits de chacun sont garantis
 2. Mission : comprendre et accompagner avec humanité et proximité
@@ -1227,20 +1252,20 @@
 4. Résultat d'ateliers de co-construction</t>
         </is>
       </c>
-      <c r="G9" s="5" t="inlineStr">
+      <c r="L9" s="5" t="inlineStr">
         <is>
           <t>Le manifeste du notariat définit une vision (croire en une société apaisée dans laquelle chacun peut compter sur le fait que ses droits sont garantis) et une mission (comprendre et accompagner avec humanité et proximité tous les citoyens à toutes les étapes de leur vie). Ces objectifs ont été définis lors d'ateliers de co-construction.</t>
         </is>
       </c>
-      <c r="H9" s="6" t="n"/>
-      <c r="I9" s="5" t="n"/>
-      <c r="J9" s="6" t="n"/>
-      <c r="K9" s="5" t="n"/>
-      <c r="L9" s="6" t="n"/>
-      <c r="M9" s="5" t="n"/>
-      <c r="N9" s="7" t="n"/>
-      <c r="O9" s="7" t="n"/>
+      <c r="M9" s="6" t="n"/>
+      <c r="N9" s="5" t="n"/>
+      <c r="O9" s="6" t="n"/>
       <c r="P9" s="5" t="n"/>
+      <c r="Q9" s="6" t="n"/>
+      <c r="R9" s="5" t="n"/>
+      <c r="S9" s="7" t="n"/>
+      <c r="T9" s="7" t="n"/>
+      <c r="U9" s="5" t="n"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="5" t="inlineStr">
@@ -1258,17 +1283,17 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="D10" s="5" t="inlineStr">
+      <c r="I10" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="E10" s="5" t="inlineStr">
+      <c r="J10" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_</t>
         </is>
       </c>
-      <c r="F10" s="5" t="inlineStr">
+      <c r="K10" s="5" t="inlineStr">
         <is>
           <t>1. Convention Collective Nationale du Notariat
 2. IDCC 2205
@@ -1276,20 +1301,20 @@
 4. Entre employeurs (notaires) et salariés</t>
         </is>
       </c>
-      <c r="G10" s="5" t="inlineStr">
+      <c r="L10" s="5" t="inlineStr">
         <is>
           <t>La CCN est la Convention Collective Nationale du Notariat, identifiée sous le code IDCC 2205. C'est le texte qui régit les relations de travail entre les employeurs (notaires) et les salariés de la profession notariale.</t>
         </is>
       </c>
-      <c r="H10" s="6" t="n"/>
-      <c r="I10" s="5" t="n"/>
-      <c r="J10" s="6" t="n"/>
-      <c r="K10" s="5" t="n"/>
-      <c r="L10" s="6" t="n"/>
-      <c r="M10" s="5" t="n"/>
-      <c r="N10" s="7" t="n"/>
-      <c r="O10" s="7" t="n"/>
+      <c r="M10" s="6" t="n"/>
+      <c r="N10" s="5" t="n"/>
+      <c r="O10" s="6" t="n"/>
       <c r="P10" s="5" t="n"/>
+      <c r="Q10" s="6" t="n"/>
+      <c r="R10" s="5" t="n"/>
+      <c r="S10" s="7" t="n"/>
+      <c r="T10" s="7" t="n"/>
+      <c r="U10" s="5" t="n"/>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="5" t="inlineStr">
@@ -1307,17 +1332,17 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="D11" s="5" t="inlineStr">
+      <c r="I11" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="E11" s="5" t="inlineStr">
+      <c r="J11" s="5" t="inlineStr">
         <is>
           <t>csn2019_avenant_n_38_opco</t>
         </is>
       </c>
-      <c r="F11" s="5" t="inlineStr">
+      <c r="K11" s="5" t="inlineStr">
         <is>
           <t>1. Opérateur de Compétences
 2. Financement de l'apprentissage et de la formation professionnelle
@@ -1325,20 +1350,20 @@
 4. Organisme agréé</t>
         </is>
       </c>
-      <c r="G11" s="5" t="inlineStr">
+      <c r="L11" s="5" t="inlineStr">
         <is>
           <t>L'OPCO (Opérateur de Compétences) est un organisme agréé pour financer l'apprentissage et la formation professionnelle. Pour le notariat, il s'agit de l'OPCO EP (Entreprises de Proximité).</t>
         </is>
       </c>
-      <c r="H11" s="6" t="n"/>
-      <c r="I11" s="5" t="n"/>
-      <c r="J11" s="6" t="n"/>
-      <c r="K11" s="5" t="n"/>
-      <c r="L11" s="6" t="n"/>
-      <c r="M11" s="5" t="n"/>
-      <c r="N11" s="7" t="n"/>
-      <c r="O11" s="7" t="n"/>
+      <c r="M11" s="6" t="n"/>
+      <c r="N11" s="5" t="n"/>
+      <c r="O11" s="6" t="n"/>
       <c r="P11" s="5" t="n"/>
+      <c r="Q11" s="6" t="n"/>
+      <c r="R11" s="5" t="n"/>
+      <c r="S11" s="7" t="n"/>
+      <c r="T11" s="7" t="n"/>
+      <c r="U11" s="5" t="n"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="5" t="inlineStr">
@@ -1356,37 +1381,37 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="D12" s="5" t="inlineStr">
+      <c r="I12" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="E12" s="5" t="inlineStr">
+      <c r="J12" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_</t>
         </is>
       </c>
-      <c r="F12" s="5" t="inlineStr">
+      <c r="K12" s="5" t="inlineStr">
         <is>
           <t>1. Article 29.5
 2. Participation financière à la formation professionnelle
 3. Date de publication : 12 décembre 2024</t>
         </is>
       </c>
-      <c r="G12" s="5" t="inlineStr">
+      <c r="L12" s="5" t="inlineStr">
         <is>
           <t>L'avenant 59 du 12 décembre 2024 a modifié l'article 29.5 de la CCN concernant la participation financière à la formation professionnelle.</t>
         </is>
       </c>
-      <c r="H12" s="6" t="n"/>
-      <c r="I12" s="5" t="n"/>
-      <c r="J12" s="6" t="n"/>
-      <c r="K12" s="5" t="n"/>
-      <c r="L12" s="6" t="n"/>
-      <c r="M12" s="5" t="n"/>
-      <c r="N12" s="7" t="n"/>
-      <c r="O12" s="7" t="n"/>
+      <c r="M12" s="6" t="n"/>
+      <c r="N12" s="5" t="n"/>
+      <c r="O12" s="6" t="n"/>
       <c r="P12" s="5" t="n"/>
+      <c r="Q12" s="6" t="n"/>
+      <c r="R12" s="5" t="n"/>
+      <c r="S12" s="7" t="n"/>
+      <c r="T12" s="7" t="n"/>
+      <c r="U12" s="5" t="n"/>
     </row>
     <row r="13" ht="60" customHeight="1">
       <c r="A13" s="5" t="inlineStr">
@@ -1404,37 +1429,37 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="D13" s="5" t="inlineStr">
+      <c r="I13" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="E13" s="5" t="inlineStr">
+      <c r="J13" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241114_avenant_58_modif_art_15_6_et_29_3_3_mis_en_forme</t>
         </is>
       </c>
-      <c r="F13" s="5" t="inlineStr">
+      <c r="K13" s="5" t="inlineStr">
         <is>
           <t>1. Article 15.6
 2. Article 29.3.3
 3. Date de publication : 14 novembre 2024</t>
         </is>
       </c>
-      <c r="G13" s="5" t="inlineStr">
+      <c r="L13" s="5" t="inlineStr">
         <is>
           <t>L'avenant 58 du 14 novembre 2024 a modifié les articles 15.6 et 29.3.3 de la CCN du notariat.</t>
         </is>
       </c>
-      <c r="H13" s="6" t="n"/>
-      <c r="I13" s="5" t="n"/>
-      <c r="J13" s="6" t="n"/>
-      <c r="K13" s="5" t="n"/>
-      <c r="L13" s="6" t="n"/>
-      <c r="M13" s="5" t="n"/>
-      <c r="N13" s="7" t="n"/>
-      <c r="O13" s="7" t="n"/>
+      <c r="M13" s="6" t="n"/>
+      <c r="N13" s="5" t="n"/>
+      <c r="O13" s="6" t="n"/>
       <c r="P13" s="5" t="n"/>
+      <c r="Q13" s="6" t="n"/>
+      <c r="R13" s="5" t="n"/>
+      <c r="S13" s="7" t="n"/>
+      <c r="T13" s="7" t="n"/>
+      <c r="U13" s="5" t="n"/>
     </row>
     <row r="14" ht="60" customHeight="1">
       <c r="A14" s="5" t="inlineStr">
@@ -1452,17 +1477,17 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="D14" s="5" t="inlineStr">
+      <c r="I14" s="5" t="inlineStr">
         <is>
           <t>Pointu</t>
         </is>
       </c>
-      <c r="E14" s="5" t="inlineStr">
+      <c r="J14" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_; convention_collective_20241114_avenant_58_modif_art_15_6_et_29_3_3_mis_en_forme</t>
         </is>
       </c>
-      <c r="F14" s="5" t="inlineStr">
+      <c r="K14" s="5" t="inlineStr">
         <is>
           <t>1. Avenant 59 modifie l'avenant 58
 2. Les deux concernent la formation professionnelle (article 29)
@@ -1470,20 +1495,20 @@
 4. Publiés à un mois d'intervalle (novembre et décembre 2024)</t>
         </is>
       </c>
-      <c r="G14" s="5" t="inlineStr">
+      <c r="L14" s="5" t="inlineStr">
         <is>
           <t>L'avenant 59 (décembre 2024) modifie l'avenant 58 (novembre 2024). Les deux avenants concernent la formation professionnelle via l'article 29 de la CCN, constituant une suite logique de modifications publiées à un mois d'intervalle.</t>
         </is>
       </c>
-      <c r="H14" s="6" t="n"/>
-      <c r="I14" s="5" t="n"/>
-      <c r="J14" s="6" t="n"/>
-      <c r="K14" s="5" t="n"/>
-      <c r="L14" s="6" t="n"/>
-      <c r="M14" s="5" t="n"/>
-      <c r="N14" s="7" t="n"/>
-      <c r="O14" s="7" t="n"/>
+      <c r="M14" s="6" t="n"/>
+      <c r="N14" s="5" t="n"/>
+      <c r="O14" s="6" t="n"/>
       <c r="P14" s="5" t="n"/>
+      <c r="Q14" s="6" t="n"/>
+      <c r="R14" s="5" t="n"/>
+      <c r="S14" s="7" t="n"/>
+      <c r="T14" s="7" t="n"/>
+      <c r="U14" s="5" t="n"/>
     </row>
     <row r="15" ht="60" customHeight="1">
       <c r="A15" s="5" t="inlineStr">
@@ -1501,17 +1526,17 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="D15" s="5" t="inlineStr">
+      <c r="I15" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="E15" s="5" t="inlineStr">
+      <c r="J15" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_; convention_collective_20241114_avenant_58_modif_art_15_6_et_29_3_3_mis_en_forme</t>
         </is>
       </c>
-      <c r="F15" s="5" t="inlineStr">
+      <c r="K15" s="5" t="inlineStr">
         <is>
           <t>1. Organisations syndicales de salariés
 2. Organisations patronales (notaires employeurs)
@@ -1520,20 +1545,20 @@
 5. Fédération générale des clercs et employés de notaire</t>
         </is>
       </c>
-      <c r="G15" s="5" t="inlineStr">
+      <c r="L15" s="5" t="inlineStr">
         <is>
           <t>Les partenaires sociaux signataires des avenants à la CCN incluent les organisations syndicales de salariés (CFE-CGC, CFTC, Fédération générale des clercs et employés de notaire) et les organisations patronales représentant les notaires employeurs.</t>
         </is>
       </c>
-      <c r="H15" s="6" t="n"/>
-      <c r="I15" s="5" t="n"/>
-      <c r="J15" s="6" t="n"/>
-      <c r="K15" s="5" t="n"/>
-      <c r="L15" s="6" t="n"/>
-      <c r="M15" s="5" t="n"/>
-      <c r="N15" s="7" t="n"/>
-      <c r="O15" s="7" t="n"/>
+      <c r="M15" s="6" t="n"/>
+      <c r="N15" s="5" t="n"/>
+      <c r="O15" s="6" t="n"/>
       <c r="P15" s="5" t="n"/>
+      <c r="Q15" s="6" t="n"/>
+      <c r="R15" s="5" t="n"/>
+      <c r="S15" s="7" t="n"/>
+      <c r="T15" s="7" t="n"/>
+      <c r="U15" s="5" t="n"/>
     </row>
     <row r="16" ht="60" customHeight="1">
       <c r="A16" s="5" t="inlineStr">
@@ -1551,17 +1576,17 @@
           <t>Edge_Case</t>
         </is>
       </c>
-      <c r="D16" s="5" t="inlineStr">
+      <c r="I16" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="E16" s="5" t="inlineStr">
+      <c r="J16" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_; convention_collective_20241114_avenant_58_modif_art_15_6_et_29_3_3_mis_en_forme; convention_collective_20240321_avenant_n56_ccn_modification_art_12_2_procedure_licenciement_mis_en_f</t>
         </is>
       </c>
-      <c r="F16" s="5" t="inlineStr">
+      <c r="K16" s="5" t="inlineStr">
         <is>
           <t>1. Avenant 56 (mars 2024) : article 12.2 sur la procédure de licenciement
 2. Avenant 58 (novembre 2024) : articles 15.6 et 29.3.3
@@ -1569,20 +1594,20 @@
 4. Questions temporelles nécessitant synthèse de plusieurs documents</t>
         </is>
       </c>
-      <c r="G16" s="5" t="inlineStr">
+      <c r="L16" s="5" t="inlineStr">
         <is>
           <t>En 2024, la CCN a connu trois modifications majeures via les avenants 56 (mars, procédure licenciement), 58 (novembre, catégories employés et formation) et 59 (décembre, participation financière formation). Ces avenants ont principalement porté sur les articles 12.2, 15.6, 29.3.3 et 29.5.</t>
         </is>
       </c>
-      <c r="H16" s="6" t="n"/>
-      <c r="I16" s="5" t="n"/>
-      <c r="J16" s="6" t="n"/>
-      <c r="K16" s="5" t="n"/>
-      <c r="L16" s="6" t="n"/>
-      <c r="M16" s="5" t="n"/>
-      <c r="N16" s="7" t="n"/>
-      <c r="O16" s="7" t="n"/>
+      <c r="M16" s="6" t="n"/>
+      <c r="N16" s="5" t="n"/>
+      <c r="O16" s="6" t="n"/>
       <c r="P16" s="5" t="n"/>
+      <c r="Q16" s="6" t="n"/>
+      <c r="R16" s="5" t="n"/>
+      <c r="S16" s="7" t="n"/>
+      <c r="T16" s="7" t="n"/>
+      <c r="U16" s="5" t="n"/>
     </row>
     <row r="17" ht="60" customHeight="1">
       <c r="A17" s="5" t="inlineStr">
@@ -1600,17 +1625,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="D17" s="5" t="inlineStr">
+      <c r="I17" s="5" t="inlineStr">
         <is>
           <t>Pointu</t>
         </is>
       </c>
-      <c r="E17" s="5" t="inlineStr">
+      <c r="J17" s="5" t="inlineStr">
         <is>
           <t>fil_infos_fil_info_262; rpn_rpn</t>
         </is>
       </c>
-      <c r="F17" s="5" t="inlineStr">
+      <c r="K17" s="5" t="inlineStr">
         <is>
           <t>1. Passage d'un règlement national-règlement intercours à un Code + RPN
 2. Séparation Code déontologie / Règlement professionnel
@@ -1619,20 +1644,20 @@
 5. Élaboration à quatre mains (profession + DACS)</t>
         </is>
       </c>
-      <c r="G17" s="5" t="inlineStr">
+      <c r="L17" s="5" t="inlineStr">
         <is>
           <t>La réforme 2021-2024 a remplacé l'ancien règlement national-règlement intercours par deux textes distincts : un Code de déontologie édicté par décret en Conseil d'État et un RPN approuvé par arrêté. Cette architecture donne une plus grande force juridique aux règles déontologiques et lie explicitement déontologie et discipline.</t>
         </is>
       </c>
-      <c r="H17" s="6" t="n"/>
-      <c r="I17" s="5" t="n"/>
-      <c r="J17" s="6" t="n"/>
-      <c r="K17" s="5" t="n"/>
-      <c r="L17" s="6" t="n"/>
-      <c r="M17" s="5" t="n"/>
-      <c r="N17" s="7" t="n"/>
-      <c r="O17" s="7" t="n"/>
+      <c r="M17" s="6" t="n"/>
+      <c r="N17" s="5" t="n"/>
+      <c r="O17" s="6" t="n"/>
       <c r="P17" s="5" t="n"/>
+      <c r="Q17" s="6" t="n"/>
+      <c r="R17" s="5" t="n"/>
+      <c r="S17" s="7" t="n"/>
+      <c r="T17" s="7" t="n"/>
+      <c r="U17" s="5" t="n"/>
     </row>
     <row r="18" ht="60" customHeight="1">
       <c r="A18" s="5" t="inlineStr">
@@ -1650,13 +1675,13 @@
           <t>Edge_Case</t>
         </is>
       </c>
-      <c r="D18" s="5" t="inlineStr">
+      <c r="I18" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="E18" s="5" t="inlineStr"/>
-      <c r="F18" s="5" t="inlineStr">
+      <c r="J18" s="5" t="inlineStr"/>
+      <c r="K18" s="5" t="inlineStr">
         <is>
           <t>1. Question hors périmètre de la Bible Notariale
 2. Concerne le parcours de formation
@@ -1664,20 +1689,20 @@
 4. Le chatbot devrait l'indiquer clairement</t>
         </is>
       </c>
-      <c r="G18" s="5" t="inlineStr">
+      <c r="L18" s="5" t="inlineStr">
         <is>
           <t>Cette question concerne le parcours de formation pour devenir notaire, ce qui est hors du périmètre des documents de la Bible Notariale qui se concentrent sur la déontologie, la CCN et les règles professionnelles pour les notaires en exercice. Le chatbot devrait indiquer qu'il ne dispose pas d'informations sur ce sujet.</t>
         </is>
       </c>
-      <c r="H18" s="6" t="n"/>
-      <c r="I18" s="5" t="n"/>
-      <c r="J18" s="6" t="n"/>
-      <c r="K18" s="5" t="n"/>
-      <c r="L18" s="6" t="n"/>
-      <c r="M18" s="5" t="n"/>
-      <c r="N18" s="7" t="n"/>
-      <c r="O18" s="7" t="n"/>
+      <c r="M18" s="6" t="n"/>
+      <c r="N18" s="5" t="n"/>
+      <c r="O18" s="6" t="n"/>
       <c r="P18" s="5" t="n"/>
+      <c r="Q18" s="6" t="n"/>
+      <c r="R18" s="5" t="n"/>
+      <c r="S18" s="7" t="n"/>
+      <c r="T18" s="7" t="n"/>
+      <c r="U18" s="5" t="n"/>
     </row>
     <row r="19" ht="60" customHeight="1">
       <c r="A19" s="5" t="inlineStr">
@@ -1695,13 +1720,13 @@
           <t>Edge_Case</t>
         </is>
       </c>
-      <c r="D19" s="5" t="inlineStr">
+      <c r="I19" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="E19" s="5" t="inlineStr"/>
-      <c r="F19" s="5" t="inlineStr">
+      <c r="J19" s="5" t="inlineStr"/>
+      <c r="K19" s="5" t="inlineStr">
         <is>
           <t>1. Question très large et historique
 2. Hors périmètre de la Bible Notariale
@@ -1709,20 +1734,20 @@
 4. Le chatbot devrait l'indiquer</t>
         </is>
       </c>
-      <c r="G19" s="5" t="inlineStr">
+      <c r="L19" s="5" t="inlineStr">
         <is>
           <t>Cette question sur l'histoire du notariat est trop large et hors du périmètre des documents de la Bible Notariale qui se concentrent sur l'actualité professionnelle, la déontologie actuelle et les règles en vigueur. Le chatbot devrait indiquer qu'il ne dispose pas d'informations historiques détaillées.</t>
         </is>
       </c>
-      <c r="H19" s="6" t="n"/>
-      <c r="I19" s="5" t="n"/>
-      <c r="J19" s="6" t="n"/>
-      <c r="K19" s="5" t="n"/>
-      <c r="L19" s="6" t="n"/>
-      <c r="M19" s="5" t="n"/>
-      <c r="N19" s="7" t="n"/>
-      <c r="O19" s="7" t="n"/>
+      <c r="M19" s="6" t="n"/>
+      <c r="N19" s="5" t="n"/>
+      <c r="O19" s="6" t="n"/>
       <c r="P19" s="5" t="n"/>
+      <c r="Q19" s="6" t="n"/>
+      <c r="R19" s="5" t="n"/>
+      <c r="S19" s="7" t="n"/>
+      <c r="T19" s="7" t="n"/>
+      <c r="U19" s="5" t="n"/>
     </row>
     <row r="20" ht="60" customHeight="1">
       <c r="A20" s="5" t="inlineStr">
@@ -1740,17 +1765,17 @@
           <t>Edge_Case</t>
         </is>
       </c>
-      <c r="D20" s="5" t="inlineStr">
+      <c r="I20" s="5" t="inlineStr">
         <is>
           <t>Pointu</t>
         </is>
       </c>
-      <c r="E20" s="5" t="inlineStr">
+      <c r="J20" s="5" t="inlineStr">
         <is>
           <t>fil_infos_fil_info_262; rpn_rpn; convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_; convention_collective_20241114_avenant_58_modif_art_15_6_et_29_3_3_mis_en_forme</t>
         </is>
       </c>
-      <c r="F20" s="5" t="inlineStr">
+      <c r="K20" s="5" t="inlineStr">
         <is>
           <t>1. Réforme déontologie : nouvelles exigences professionnelles
 2. CCN formation : mise en conformité avec obligations
@@ -1758,20 +1783,20 @@
 4. Période de transformation 2021-2024</t>
         </is>
       </c>
-      <c r="G20" s="5" t="inlineStr">
+      <c r="L20" s="5" t="inlineStr">
         <is>
           <t>La réforme de la déontologie (2021-2024) a établi de nouvelles exigences professionnelles, tandis que les modifications de la CCN sur la formation (avenants 58-59 en 2024) ont mis à jour les modalités de formation pour s'aligner sur ces nouvelles obligations. Ces évolutions parallèles illustrent la cohérence entre textes déontologiques et sociaux.</t>
         </is>
       </c>
-      <c r="H20" s="6" t="n"/>
-      <c r="I20" s="5" t="n"/>
-      <c r="J20" s="6" t="n"/>
-      <c r="K20" s="5" t="n"/>
-      <c r="L20" s="6" t="n"/>
-      <c r="M20" s="5" t="n"/>
-      <c r="N20" s="7" t="n"/>
-      <c r="O20" s="7" t="n"/>
+      <c r="M20" s="6" t="n"/>
+      <c r="N20" s="5" t="n"/>
+      <c r="O20" s="6" t="n"/>
       <c r="P20" s="5" t="n"/>
+      <c r="Q20" s="6" t="n"/>
+      <c r="R20" s="5" t="n"/>
+      <c r="S20" s="7" t="n"/>
+      <c r="T20" s="7" t="n"/>
+      <c r="U20" s="5" t="n"/>
     </row>
     <row r="21" ht="60" customHeight="1">
       <c r="A21" s="5" t="inlineStr">
@@ -1789,17 +1814,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="D21" s="5" t="inlineStr">
+      <c r="I21" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="E21" s="5" t="inlineStr">
+      <c r="J21" s="5" t="inlineStr">
         <is>
           <t>rpn_rpn</t>
         </is>
       </c>
-      <c r="F21" s="5" t="inlineStr">
+      <c r="K21" s="5" t="inlineStr">
         <is>
           <t>1. Original de l'acte authentique
 2. Conservé par le notaire
@@ -1807,23 +1832,23 @@
 4. Seules des copies (expéditions) sont délivrées</t>
         </is>
       </c>
-      <c r="G21" s="5" t="inlineStr">
+      <c r="L21" s="5" t="inlineStr">
         <is>
           <t>La minute est l'original d'un acte authentique conservé par le notaire. C'est un document source qui ne peut quitter l'étude et dont seules des copies appelées expéditions sont délivrées aux parties.</t>
         </is>
       </c>
-      <c r="H21" s="6" t="n"/>
-      <c r="I21" s="5" t="n"/>
-      <c r="J21" s="6" t="n"/>
-      <c r="K21" s="5" t="n"/>
-      <c r="L21" s="6" t="n"/>
-      <c r="M21" s="5" t="n"/>
-      <c r="N21" s="7" t="n"/>
-      <c r="O21" s="7" t="n"/>
+      <c r="M21" s="6" t="n"/>
+      <c r="N21" s="5" t="n"/>
+      <c r="O21" s="6" t="n"/>
       <c r="P21" s="5" t="n"/>
+      <c r="Q21" s="6" t="n"/>
+      <c r="R21" s="5" t="n"/>
+      <c r="S21" s="7" t="n"/>
+      <c r="T21" s="7" t="n"/>
+      <c r="U21" s="5" t="n"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="9">
     <dataValidation sqref="H2:H21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Valeur invalide" error="Veuillez choisir une valeur dans la liste" type="list">
       <formula1>"Oui,Non,A reformuler"</formula1>
     </dataValidation>
@@ -1836,7 +1861,712 @@
     <dataValidation sqref="N2:N21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Valeur invalide" error="Veuillez choisir une valeur dans la liste" type="list">
       <formula1>"Oui,Non,A preciser"</formula1>
     </dataValidation>
+    <dataValidation sqref="D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" promptTitle="Type de document" prompt="Choisissez un type de document" type="list">
+      <formula1>=Ref_TypesDocument!$A$2:$A$6</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2 E3 E4 E5 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" promptTitle="Domaine métier" prompt="Choisissez un domaine métier" type="list">
+      <formula1>=Ref_DomainesMetier!$A$2:$A$4</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2 F3 F4 F5 F6 F7 F8 F9 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" promptTitle="Source de document" prompt="Choisissez une source de document" type="list">
+      <formula1>=Ref_SourcesDocument!$A$2:$A$9</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2 G3 G4 G5 G6 G7 G8 G9 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" promptTitle="Thématiques" prompt="Choisissez une ou plusieurs thématiques (séparées par des virgules)" type="list">
+      <formula1>=Ref_Thematiques!$A$2:$A$20</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" promptTitle="Mots-clés" prompt="Choisissez un ou plusieurs mots-clés (séparés par des virgules)" type="list">
+      <formula1>=Ref_MotsCles!$A$2:$A$46</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Type de document</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Actualités</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Assurances</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Convention collectives Notariat</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Directives CSN</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Lois et règlements</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Thématique</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>acte authentique</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>avenant</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>circulaire</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>congés payés</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>conseil supérieur du notariat</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>convention collective</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>cybersécurité</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>formation professionnelle</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>harcèlement</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>intéressement</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>lcb-ft</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>licenciement</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>minute</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>opco</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>prévoyance</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>rgpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>rémunération</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>tarification</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>égalité professionnelle</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Mot-clé</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CRIDON</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FAQ notariale</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>actualité juridique</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>administration</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>assurance professionnelle</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>base de connaissances</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>bonnes pratiques</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>carrière notaire</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>circulaire CSN</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>complémentaire santé</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>conformité</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>congés payés</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>consultation juridique</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>convention collective</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>cyber-risques</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>cybersécurité</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>doctrine</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>documentation</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>documentation métier</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>droit social</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>déclarations</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>expertise notariale</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>formation</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>formation professionnelle</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>harcèlement au travail</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>instructions professionnelles</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>législation</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>négociation collective</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>obligations fiscales</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>parcours professionnel</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>participation aux bénéfices</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>procédure disciplinaire</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>protection des données</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>protection données</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>prévention harcèlement</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>prévoyance</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>questions-réponses</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>recherche juridique</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>responsabilité civile</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>réglementation notariale</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>rémunération</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>textes réglementaires</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>transactions immobilières</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>veille professionnelle</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>égalité professionnelle</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Source de document</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>accord_branche</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>assurance</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>avenant_ccn</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>circulaire_csn</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>conformite</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>decret_ordonnance</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fil_info</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>guide_pratique</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Domaine métier</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ASSURANCES</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DEONTOLOGIE</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>RH</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correction : ajout de colonnes multiples pour thématiques et mots-clés
## Problème résolu

Excel ne permet qu'une seule sélection par liste déroulante.

## Solution

**Au lieu de :**
- 1 colonne Thematiques
- 1 colonne Mots_Cles

**Maintenant :**
- 3 colonnes : Thematique_1, Thematique_2, Thematique_3
- 3 colonnes : Mot_Cle_1, Mot_Cle_2, Mot_Cle_3

Chaque colonne a sa propre liste déroulante, permettant de sélectionner
jusqu'à 3 thématiques et 3 mots-clés par question.

## Structure finale

**9 nouvelles colonnes** (au lieu de 5) :
1. Type_Document (1 sélection)
2. Domaine_Metier (1 sélection)
3. Source_Document (1 sélection)
4-6. Thematique_1/2/3 (3 sélections possibles)
7-9. Mot_Cle_1/2/3 (3 sélections possibles)

Total colonnes : 25 (au lieu de 21)

**Fichiers modifiés :**
- update_validation_dataset.py : logique adaptée
- output/validation_dataset_20questions.xlsx : régénéré
</commit_message>
<xml_diff>
--- a/output/validation_dataset_20questions.xlsx
+++ b/output/validation_dataset_20questions.xlsx
@@ -741,7 +741,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -803,75 +803,95 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Thematiques</t>
+          <t>Thematique_1</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Mots_Cles</t>
-        </is>
-      </c>
-      <c r="I1" s="4" t="inlineStr">
+          <t>Thematique_2</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Thematique_3</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Mot_Cle_1</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Mot_Cle_2</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Mot_Cle_3</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>Difficulte</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>Documents_Sources_Proposes</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>Elements_Cles_Reponse</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>Reponse_Attendue_Resumee</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>Validation_Question</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>Correction_Question</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>Validation_Sources</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>Correction_Sources</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="U1" s="4" t="inlineStr">
         <is>
           <t>Validation_Elements_Cles</t>
         </is>
       </c>
-      <c r="R1" s="4" t="inlineStr">
+      <c r="V1" s="4" t="inlineStr">
         <is>
           <t>Correction_Elements_Cles</t>
         </is>
       </c>
-      <c r="S1" s="4" t="inlineStr">
+      <c r="W1" s="4" t="inlineStr">
         <is>
           <t>Validation_Reponse_Attendue</t>
         </is>
       </c>
-      <c r="T1" s="4" t="inlineStr">
+      <c r="X1" s="4" t="inlineStr">
         <is>
           <t>Correction_Reponse_Attendue</t>
         </is>
       </c>
-      <c r="U1" s="4" t="inlineStr">
+      <c r="Y1" s="4" t="inlineStr">
         <is>
           <t>Commentaires</t>
         </is>
@@ -893,37 +913,37 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="M2" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="J2" s="5" t="inlineStr">
+      <c r="N2" s="5" t="inlineStr">
         <is>
           <t>csn2019_analyse_nationale_des_risques_lcb_ft_en_france_septembre_2019</t>
         </is>
       </c>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="O2" s="5" t="inlineStr">
         <is>
           <t>1. Lutte Contre le Blanchiment de capitaux
 2. Financement du Terrorisme
 3. Obligation légale pour les notaires</t>
         </is>
       </c>
-      <c r="L2" s="5" t="inlineStr">
+      <c r="P2" s="5" t="inlineStr">
         <is>
           <t>LCB-FT signifie Lutte Contre le Blanchiment de capitaux et le Financement du Terrorisme. Il s'agit d'un ensemble d'obligations légales imposées aux notaires pour prévenir l'utilisation du système financier à des fins illégales.</t>
         </is>
       </c>
-      <c r="M2" s="6" t="n"/>
-      <c r="N2" s="5" t="n"/>
-      <c r="O2" s="6" t="n"/>
-      <c r="P2" s="5" t="n"/>
       <c r="Q2" s="6" t="n"/>
       <c r="R2" s="5" t="n"/>
-      <c r="S2" s="7" t="n"/>
-      <c r="T2" s="7" t="n"/>
-      <c r="U2" s="5" t="n"/>
+      <c r="S2" s="6" t="n"/>
+      <c r="T2" s="5" t="n"/>
+      <c r="U2" s="6" t="n"/>
+      <c r="V2" s="5" t="n"/>
+      <c r="W2" s="7" t="n"/>
+      <c r="X2" s="7" t="n"/>
+      <c r="Y2" s="5" t="n"/>
     </row>
     <row r="3" ht="60" customHeight="1">
       <c r="A3" s="5" t="inlineStr">
@@ -941,37 +961,37 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="M3" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="N3" s="5" t="inlineStr">
         <is>
           <t>rpn_rpn</t>
         </is>
       </c>
-      <c r="K3" s="5" t="inlineStr">
+      <c r="O3" s="5" t="inlineStr">
         <is>
           <t>1. Règlement Professionnel du Notariat
 2. Entré en vigueur le 1er février 2024
 3. Approuvé par arrêté du Garde des Sceaux du 29 janvier 2024</t>
         </is>
       </c>
-      <c r="L3" s="5" t="inlineStr">
+      <c r="P3" s="5" t="inlineStr">
         <is>
           <t>Le RPN est le Règlement Professionnel du Notariat. Il est entré en vigueur le 1er février 2024 après avoir été approuvé par arrêté du Garde des Sceaux en date du 29 janvier 2024. Il remplace l'ancien règlement national-règlement intercours.</t>
         </is>
       </c>
-      <c r="M3" s="6" t="n"/>
-      <c r="N3" s="5" t="n"/>
-      <c r="O3" s="6" t="n"/>
-      <c r="P3" s="5" t="n"/>
       <c r="Q3" s="6" t="n"/>
       <c r="R3" s="5" t="n"/>
-      <c r="S3" s="7" t="n"/>
-      <c r="T3" s="7" t="n"/>
-      <c r="U3" s="5" t="n"/>
+      <c r="S3" s="6" t="n"/>
+      <c r="T3" s="5" t="n"/>
+      <c r="U3" s="6" t="n"/>
+      <c r="V3" s="5" t="n"/>
+      <c r="W3" s="7" t="n"/>
+      <c r="X3" s="7" t="n"/>
+      <c r="Y3" s="5" t="n"/>
     </row>
     <row r="4" ht="60" customHeight="1">
       <c r="A4" s="5" t="inlineStr">
@@ -989,37 +1009,37 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="I4" s="5" t="inlineStr">
+      <c r="M4" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="J4" s="5" t="inlineStr">
+      <c r="N4" s="5" t="inlineStr">
         <is>
           <t>rpn_rpn; fil_infos_fil_info_262</t>
         </is>
       </c>
-      <c r="K4" s="5" t="inlineStr">
+      <c r="O4" s="5" t="inlineStr">
         <is>
           <t>1. 1er février 2024
 2. Décret du 28 décembre 2023
 3. En même temps que le RPN</t>
         </is>
       </c>
-      <c r="L4" s="5" t="inlineStr">
+      <c r="P4" s="5" t="inlineStr">
         <is>
           <t>Le Code de déontologie des notaires est entré en vigueur le 1er février 2024, édicté par décret du 28 décembre 2023, en même temps que le Règlement Professionnel du Notariat (RPN).</t>
         </is>
       </c>
-      <c r="M4" s="6" t="n"/>
-      <c r="N4" s="5" t="n"/>
-      <c r="O4" s="6" t="n"/>
-      <c r="P4" s="5" t="n"/>
       <c r="Q4" s="6" t="n"/>
       <c r="R4" s="5" t="n"/>
-      <c r="S4" s="7" t="n"/>
-      <c r="T4" s="7" t="n"/>
-      <c r="U4" s="5" t="n"/>
+      <c r="S4" s="6" t="n"/>
+      <c r="T4" s="5" t="n"/>
+      <c r="U4" s="6" t="n"/>
+      <c r="V4" s="5" t="n"/>
+      <c r="W4" s="7" t="n"/>
+      <c r="X4" s="7" t="n"/>
+      <c r="Y4" s="5" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
       <c r="A5" s="5" t="inlineStr">
@@ -1037,37 +1057,37 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="I5" s="5" t="inlineStr">
+      <c r="M5" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="J5" s="5" t="inlineStr">
+      <c r="N5" s="5" t="inlineStr">
         <is>
           <t>fil_infos_fil_info_262</t>
         </is>
       </c>
-      <c r="K5" s="5" t="inlineStr">
+      <c r="O5" s="5" t="inlineStr">
         <is>
           <t>1. Loi du 18 novembre 2021 pour la confiance dans l'institution judiciaire
 2. Ordonnance du 13 avril 2022
 3. Réforme profonde de la discipline et de la déontologie</t>
         </is>
       </c>
-      <c r="L5" s="5" t="inlineStr">
+      <c r="P5" s="5" t="inlineStr">
         <is>
           <t>La loi du 18 novembre 2021 pour la confiance dans l'institution judiciaire et l'ordonnance du 13 avril 2022 ont réformé en profondeur la discipline et la déontologie notariale. Ces textes sont applicables à l'action des professionnels du droit, donc aux notaires.</t>
         </is>
       </c>
-      <c r="M5" s="6" t="n"/>
-      <c r="N5" s="5" t="n"/>
-      <c r="O5" s="6" t="n"/>
-      <c r="P5" s="5" t="n"/>
       <c r="Q5" s="6" t="n"/>
       <c r="R5" s="5" t="n"/>
-      <c r="S5" s="7" t="n"/>
-      <c r="T5" s="7" t="n"/>
-      <c r="U5" s="5" t="n"/>
+      <c r="S5" s="6" t="n"/>
+      <c r="T5" s="5" t="n"/>
+      <c r="U5" s="6" t="n"/>
+      <c r="V5" s="5" t="n"/>
+      <c r="W5" s="7" t="n"/>
+      <c r="X5" s="7" t="n"/>
+      <c r="Y5" s="5" t="n"/>
     </row>
     <row r="6" ht="60" customHeight="1">
       <c r="A6" s="5" t="inlineStr">
@@ -1085,17 +1105,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="I6" s="5" t="inlineStr">
+      <c r="M6" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="J6" s="5" t="inlineStr">
+      <c r="N6" s="5" t="inlineStr">
         <is>
           <t>csn2019_analyse_nationale_des_risques_lcb_ft_en_france_septembre_2019</t>
         </is>
       </c>
-      <c r="K6" s="5" t="inlineStr">
+      <c r="O6" s="5" t="inlineStr">
         <is>
           <t>1. Obligation devenue pratique professionnelle quotidienne
 2. Premiers contributeurs du secteur non-financier
@@ -1103,20 +1123,20 @@
 4. Prévenir le blanchiment de capitaux</t>
         </is>
       </c>
-      <c r="L6" s="5" t="inlineStr">
+      <c r="P6" s="5" t="inlineStr">
         <is>
           <t>Le notariat remplit un rôle important dans la LCB-FT qui est devenue une pratique professionnelle quotidienne. Les notaires sont les premiers contributeurs du secteur non-financier auprès du service de renseignement gouvernemental Tracfin, avec pour mission de prévenir l'utilisation du système financier à des fins de blanchiment.</t>
         </is>
       </c>
-      <c r="M6" s="6" t="n"/>
-      <c r="N6" s="5" t="n"/>
-      <c r="O6" s="6" t="n"/>
-      <c r="P6" s="5" t="n"/>
       <c r="Q6" s="6" t="n"/>
       <c r="R6" s="5" t="n"/>
-      <c r="S6" s="7" t="n"/>
-      <c r="T6" s="7" t="n"/>
-      <c r="U6" s="5" t="n"/>
+      <c r="S6" s="6" t="n"/>
+      <c r="T6" s="5" t="n"/>
+      <c r="U6" s="6" t="n"/>
+      <c r="V6" s="5" t="n"/>
+      <c r="W6" s="7" t="n"/>
+      <c r="X6" s="7" t="n"/>
+      <c r="Y6" s="5" t="n"/>
     </row>
     <row r="7" ht="60" customHeight="1">
       <c r="A7" s="5" t="inlineStr">
@@ -1134,17 +1154,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="I7" s="5" t="inlineStr">
+      <c r="M7" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="J7" s="5" t="inlineStr">
+      <c r="N7" s="5" t="inlineStr">
         <is>
           <t>rpn_rpn</t>
         </is>
       </c>
-      <c r="K7" s="5" t="inlineStr">
+      <c r="O7" s="5" t="inlineStr">
         <is>
           <t>1. Acte reçu par un officier public (notaire)
 2. Confère foi publique à son contenu
@@ -1152,20 +1172,20 @@
 4. Force exécutoire</t>
         </is>
       </c>
-      <c r="L7" s="5" t="inlineStr">
+      <c r="P7" s="5" t="inlineStr">
         <is>
           <t>Un acte authentique est un acte reçu par un officier public, en l'occurrence le notaire, qui confère foi publique à son contenu. Il a une date certaine et possède une force exécutoire, ce qui lui donne une valeur juridique particulière.</t>
         </is>
       </c>
-      <c r="M7" s="6" t="n"/>
-      <c r="N7" s="5" t="n"/>
-      <c r="O7" s="6" t="n"/>
-      <c r="P7" s="5" t="n"/>
       <c r="Q7" s="6" t="n"/>
       <c r="R7" s="5" t="n"/>
-      <c r="S7" s="7" t="n"/>
-      <c r="T7" s="7" t="n"/>
-      <c r="U7" s="5" t="n"/>
+      <c r="S7" s="6" t="n"/>
+      <c r="T7" s="5" t="n"/>
+      <c r="U7" s="6" t="n"/>
+      <c r="V7" s="5" t="n"/>
+      <c r="W7" s="7" t="n"/>
+      <c r="X7" s="7" t="n"/>
+      <c r="Y7" s="5" t="n"/>
     </row>
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="5" t="inlineStr">
@@ -1183,17 +1203,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="I8" s="5" t="inlineStr">
+      <c r="M8" s="5" t="inlineStr">
         <is>
           <t>Pointu</t>
         </is>
       </c>
-      <c r="J8" s="5" t="inlineStr">
+      <c r="N8" s="5" t="inlineStr">
         <is>
           <t>rpn_rpn</t>
         </is>
       </c>
-      <c r="K8" s="5" t="inlineStr">
+      <c r="O8" s="5" t="inlineStr">
         <is>
           <t>1. Entrés en vigueur simultanément le 1er février 2024
 2. Code de déontologie édicté par décret en Conseil d'État
@@ -1203,20 +1223,20 @@
 6. Violation expose à des poursuites disciplinaires</t>
         </is>
       </c>
-      <c r="L8" s="5" t="inlineStr">
+      <c r="P8" s="5" t="inlineStr">
         <is>
           <t>Le Code de déontologie et le RPN sont deux textes complémentaires entrés en vigueur simultanément le 1er février 2024. Le Code de déontologie, édicté par décret en Conseil d'État, pose les principes déontologiques généraux. Le RPN, approuvé par arrêté du Garde des Sceaux, détaille les règles d'application pratiques. La violation de ces dispositions expose à des poursuites disciplinaires.</t>
         </is>
       </c>
-      <c r="M8" s="6" t="n"/>
-      <c r="N8" s="5" t="n"/>
-      <c r="O8" s="6" t="n"/>
-      <c r="P8" s="5" t="n"/>
       <c r="Q8" s="6" t="n"/>
       <c r="R8" s="5" t="n"/>
-      <c r="S8" s="7" t="n"/>
-      <c r="T8" s="7" t="n"/>
-      <c r="U8" s="5" t="n"/>
+      <c r="S8" s="6" t="n"/>
+      <c r="T8" s="5" t="n"/>
+      <c r="U8" s="6" t="n"/>
+      <c r="V8" s="5" t="n"/>
+      <c r="W8" s="7" t="n"/>
+      <c r="X8" s="7" t="n"/>
+      <c r="Y8" s="5" t="n"/>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="5" t="inlineStr">
@@ -1234,17 +1254,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="I9" s="5" t="inlineStr">
+      <c r="M9" s="5" t="inlineStr">
         <is>
           <t>Pointu</t>
         </is>
       </c>
-      <c r="J9" s="5" t="inlineStr">
+      <c r="N9" s="5" t="inlineStr">
         <is>
           <t>fil_infos_fil_info_265</t>
         </is>
       </c>
-      <c r="K9" s="5" t="inlineStr">
+      <c r="O9" s="5" t="inlineStr">
         <is>
           <t>1. Vision : société apaisée où les droits de chacun sont garantis
 2. Mission : comprendre et accompagner avec humanité et proximité
@@ -1252,20 +1272,20 @@
 4. Résultat d'ateliers de co-construction</t>
         </is>
       </c>
-      <c r="L9" s="5" t="inlineStr">
+      <c r="P9" s="5" t="inlineStr">
         <is>
           <t>Le manifeste du notariat définit une vision (croire en une société apaisée dans laquelle chacun peut compter sur le fait que ses droits sont garantis) et une mission (comprendre et accompagner avec humanité et proximité tous les citoyens à toutes les étapes de leur vie). Ces objectifs ont été définis lors d'ateliers de co-construction.</t>
         </is>
       </c>
-      <c r="M9" s="6" t="n"/>
-      <c r="N9" s="5" t="n"/>
-      <c r="O9" s="6" t="n"/>
-      <c r="P9" s="5" t="n"/>
       <c r="Q9" s="6" t="n"/>
       <c r="R9" s="5" t="n"/>
-      <c r="S9" s="7" t="n"/>
-      <c r="T9" s="7" t="n"/>
-      <c r="U9" s="5" t="n"/>
+      <c r="S9" s="6" t="n"/>
+      <c r="T9" s="5" t="n"/>
+      <c r="U9" s="6" t="n"/>
+      <c r="V9" s="5" t="n"/>
+      <c r="W9" s="7" t="n"/>
+      <c r="X9" s="7" t="n"/>
+      <c r="Y9" s="5" t="n"/>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="5" t="inlineStr">
@@ -1283,17 +1303,17 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="I10" s="5" t="inlineStr">
+      <c r="M10" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="J10" s="5" t="inlineStr">
+      <c r="N10" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_</t>
         </is>
       </c>
-      <c r="K10" s="5" t="inlineStr">
+      <c r="O10" s="5" t="inlineStr">
         <is>
           <t>1. Convention Collective Nationale du Notariat
 2. IDCC 2205
@@ -1301,20 +1321,20 @@
 4. Entre employeurs (notaires) et salariés</t>
         </is>
       </c>
-      <c r="L10" s="5" t="inlineStr">
+      <c r="P10" s="5" t="inlineStr">
         <is>
           <t>La CCN est la Convention Collective Nationale du Notariat, identifiée sous le code IDCC 2205. C'est le texte qui régit les relations de travail entre les employeurs (notaires) et les salariés de la profession notariale.</t>
         </is>
       </c>
-      <c r="M10" s="6" t="n"/>
-      <c r="N10" s="5" t="n"/>
-      <c r="O10" s="6" t="n"/>
-      <c r="P10" s="5" t="n"/>
       <c r="Q10" s="6" t="n"/>
       <c r="R10" s="5" t="n"/>
-      <c r="S10" s="7" t="n"/>
-      <c r="T10" s="7" t="n"/>
-      <c r="U10" s="5" t="n"/>
+      <c r="S10" s="6" t="n"/>
+      <c r="T10" s="5" t="n"/>
+      <c r="U10" s="6" t="n"/>
+      <c r="V10" s="5" t="n"/>
+      <c r="W10" s="7" t="n"/>
+      <c r="X10" s="7" t="n"/>
+      <c r="Y10" s="5" t="n"/>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="5" t="inlineStr">
@@ -1332,17 +1352,17 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="I11" s="5" t="inlineStr">
+      <c r="M11" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="J11" s="5" t="inlineStr">
+      <c r="N11" s="5" t="inlineStr">
         <is>
           <t>csn2019_avenant_n_38_opco</t>
         </is>
       </c>
-      <c r="K11" s="5" t="inlineStr">
+      <c r="O11" s="5" t="inlineStr">
         <is>
           <t>1. Opérateur de Compétences
 2. Financement de l'apprentissage et de la formation professionnelle
@@ -1350,20 +1370,20 @@
 4. Organisme agréé</t>
         </is>
       </c>
-      <c r="L11" s="5" t="inlineStr">
+      <c r="P11" s="5" t="inlineStr">
         <is>
           <t>L'OPCO (Opérateur de Compétences) est un organisme agréé pour financer l'apprentissage et la formation professionnelle. Pour le notariat, il s'agit de l'OPCO EP (Entreprises de Proximité).</t>
         </is>
       </c>
-      <c r="M11" s="6" t="n"/>
-      <c r="N11" s="5" t="n"/>
-      <c r="O11" s="6" t="n"/>
-      <c r="P11" s="5" t="n"/>
       <c r="Q11" s="6" t="n"/>
       <c r="R11" s="5" t="n"/>
-      <c r="S11" s="7" t="n"/>
-      <c r="T11" s="7" t="n"/>
-      <c r="U11" s="5" t="n"/>
+      <c r="S11" s="6" t="n"/>
+      <c r="T11" s="5" t="n"/>
+      <c r="U11" s="6" t="n"/>
+      <c r="V11" s="5" t="n"/>
+      <c r="W11" s="7" t="n"/>
+      <c r="X11" s="7" t="n"/>
+      <c r="Y11" s="5" t="n"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="5" t="inlineStr">
@@ -1381,37 +1401,37 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="I12" s="5" t="inlineStr">
+      <c r="M12" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="J12" s="5" t="inlineStr">
+      <c r="N12" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_</t>
         </is>
       </c>
-      <c r="K12" s="5" t="inlineStr">
+      <c r="O12" s="5" t="inlineStr">
         <is>
           <t>1. Article 29.5
 2. Participation financière à la formation professionnelle
 3. Date de publication : 12 décembre 2024</t>
         </is>
       </c>
-      <c r="L12" s="5" t="inlineStr">
+      <c r="P12" s="5" t="inlineStr">
         <is>
           <t>L'avenant 59 du 12 décembre 2024 a modifié l'article 29.5 de la CCN concernant la participation financière à la formation professionnelle.</t>
         </is>
       </c>
-      <c r="M12" s="6" t="n"/>
-      <c r="N12" s="5" t="n"/>
-      <c r="O12" s="6" t="n"/>
-      <c r="P12" s="5" t="n"/>
       <c r="Q12" s="6" t="n"/>
       <c r="R12" s="5" t="n"/>
-      <c r="S12" s="7" t="n"/>
-      <c r="T12" s="7" t="n"/>
-      <c r="U12" s="5" t="n"/>
+      <c r="S12" s="6" t="n"/>
+      <c r="T12" s="5" t="n"/>
+      <c r="U12" s="6" t="n"/>
+      <c r="V12" s="5" t="n"/>
+      <c r="W12" s="7" t="n"/>
+      <c r="X12" s="7" t="n"/>
+      <c r="Y12" s="5" t="n"/>
     </row>
     <row r="13" ht="60" customHeight="1">
       <c r="A13" s="5" t="inlineStr">
@@ -1429,37 +1449,37 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="I13" s="5" t="inlineStr">
+      <c r="M13" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="J13" s="5" t="inlineStr">
+      <c r="N13" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241114_avenant_58_modif_art_15_6_et_29_3_3_mis_en_forme</t>
         </is>
       </c>
-      <c r="K13" s="5" t="inlineStr">
+      <c r="O13" s="5" t="inlineStr">
         <is>
           <t>1. Article 15.6
 2. Article 29.3.3
 3. Date de publication : 14 novembre 2024</t>
         </is>
       </c>
-      <c r="L13" s="5" t="inlineStr">
+      <c r="P13" s="5" t="inlineStr">
         <is>
           <t>L'avenant 58 du 14 novembre 2024 a modifié les articles 15.6 et 29.3.3 de la CCN du notariat.</t>
         </is>
       </c>
-      <c r="M13" s="6" t="n"/>
-      <c r="N13" s="5" t="n"/>
-      <c r="O13" s="6" t="n"/>
-      <c r="P13" s="5" t="n"/>
       <c r="Q13" s="6" t="n"/>
       <c r="R13" s="5" t="n"/>
-      <c r="S13" s="7" t="n"/>
-      <c r="T13" s="7" t="n"/>
-      <c r="U13" s="5" t="n"/>
+      <c r="S13" s="6" t="n"/>
+      <c r="T13" s="5" t="n"/>
+      <c r="U13" s="6" t="n"/>
+      <c r="V13" s="5" t="n"/>
+      <c r="W13" s="7" t="n"/>
+      <c r="X13" s="7" t="n"/>
+      <c r="Y13" s="5" t="n"/>
     </row>
     <row r="14" ht="60" customHeight="1">
       <c r="A14" s="5" t="inlineStr">
@@ -1477,17 +1497,17 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="I14" s="5" t="inlineStr">
+      <c r="M14" s="5" t="inlineStr">
         <is>
           <t>Pointu</t>
         </is>
       </c>
-      <c r="J14" s="5" t="inlineStr">
+      <c r="N14" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_; convention_collective_20241114_avenant_58_modif_art_15_6_et_29_3_3_mis_en_forme</t>
         </is>
       </c>
-      <c r="K14" s="5" t="inlineStr">
+      <c r="O14" s="5" t="inlineStr">
         <is>
           <t>1. Avenant 59 modifie l'avenant 58
 2. Les deux concernent la formation professionnelle (article 29)
@@ -1495,20 +1515,20 @@
 4. Publiés à un mois d'intervalle (novembre et décembre 2024)</t>
         </is>
       </c>
-      <c r="L14" s="5" t="inlineStr">
+      <c r="P14" s="5" t="inlineStr">
         <is>
           <t>L'avenant 59 (décembre 2024) modifie l'avenant 58 (novembre 2024). Les deux avenants concernent la formation professionnelle via l'article 29 de la CCN, constituant une suite logique de modifications publiées à un mois d'intervalle.</t>
         </is>
       </c>
-      <c r="M14" s="6" t="n"/>
-      <c r="N14" s="5" t="n"/>
-      <c r="O14" s="6" t="n"/>
-      <c r="P14" s="5" t="n"/>
       <c r="Q14" s="6" t="n"/>
       <c r="R14" s="5" t="n"/>
-      <c r="S14" s="7" t="n"/>
-      <c r="T14" s="7" t="n"/>
-      <c r="U14" s="5" t="n"/>
+      <c r="S14" s="6" t="n"/>
+      <c r="T14" s="5" t="n"/>
+      <c r="U14" s="6" t="n"/>
+      <c r="V14" s="5" t="n"/>
+      <c r="W14" s="7" t="n"/>
+      <c r="X14" s="7" t="n"/>
+      <c r="Y14" s="5" t="n"/>
     </row>
     <row r="15" ht="60" customHeight="1">
       <c r="A15" s="5" t="inlineStr">
@@ -1526,17 +1546,17 @@
           <t>Juridique</t>
         </is>
       </c>
-      <c r="I15" s="5" t="inlineStr">
+      <c r="M15" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="J15" s="5" t="inlineStr">
+      <c r="N15" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_; convention_collective_20241114_avenant_58_modif_art_15_6_et_29_3_3_mis_en_forme</t>
         </is>
       </c>
-      <c r="K15" s="5" t="inlineStr">
+      <c r="O15" s="5" t="inlineStr">
         <is>
           <t>1. Organisations syndicales de salariés
 2. Organisations patronales (notaires employeurs)
@@ -1545,20 +1565,20 @@
 5. Fédération générale des clercs et employés de notaire</t>
         </is>
       </c>
-      <c r="L15" s="5" t="inlineStr">
+      <c r="P15" s="5" t="inlineStr">
         <is>
           <t>Les partenaires sociaux signataires des avenants à la CCN incluent les organisations syndicales de salariés (CFE-CGC, CFTC, Fédération générale des clercs et employés de notaire) et les organisations patronales représentant les notaires employeurs.</t>
         </is>
       </c>
-      <c r="M15" s="6" t="n"/>
-      <c r="N15" s="5" t="n"/>
-      <c r="O15" s="6" t="n"/>
-      <c r="P15" s="5" t="n"/>
       <c r="Q15" s="6" t="n"/>
       <c r="R15" s="5" t="n"/>
-      <c r="S15" s="7" t="n"/>
-      <c r="T15" s="7" t="n"/>
-      <c r="U15" s="5" t="n"/>
+      <c r="S15" s="6" t="n"/>
+      <c r="T15" s="5" t="n"/>
+      <c r="U15" s="6" t="n"/>
+      <c r="V15" s="5" t="n"/>
+      <c r="W15" s="7" t="n"/>
+      <c r="X15" s="7" t="n"/>
+      <c r="Y15" s="5" t="n"/>
     </row>
     <row r="16" ht="60" customHeight="1">
       <c r="A16" s="5" t="inlineStr">
@@ -1576,17 +1596,17 @@
           <t>Edge_Case</t>
         </is>
       </c>
-      <c r="I16" s="5" t="inlineStr">
+      <c r="M16" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="J16" s="5" t="inlineStr">
+      <c r="N16" s="5" t="inlineStr">
         <is>
           <t>convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_; convention_collective_20241114_avenant_58_modif_art_15_6_et_29_3_3_mis_en_forme; convention_collective_20240321_avenant_n56_ccn_modification_art_12_2_procedure_licenciement_mis_en_f</t>
         </is>
       </c>
-      <c r="K16" s="5" t="inlineStr">
+      <c r="O16" s="5" t="inlineStr">
         <is>
           <t>1. Avenant 56 (mars 2024) : article 12.2 sur la procédure de licenciement
 2. Avenant 58 (novembre 2024) : articles 15.6 et 29.3.3
@@ -1594,20 +1614,20 @@
 4. Questions temporelles nécessitant synthèse de plusieurs documents</t>
         </is>
       </c>
-      <c r="L16" s="5" t="inlineStr">
+      <c r="P16" s="5" t="inlineStr">
         <is>
           <t>En 2024, la CCN a connu trois modifications majeures via les avenants 56 (mars, procédure licenciement), 58 (novembre, catégories employés et formation) et 59 (décembre, participation financière formation). Ces avenants ont principalement porté sur les articles 12.2, 15.6, 29.3.3 et 29.5.</t>
         </is>
       </c>
-      <c r="M16" s="6" t="n"/>
-      <c r="N16" s="5" t="n"/>
-      <c r="O16" s="6" t="n"/>
-      <c r="P16" s="5" t="n"/>
       <c r="Q16" s="6" t="n"/>
       <c r="R16" s="5" t="n"/>
-      <c r="S16" s="7" t="n"/>
-      <c r="T16" s="7" t="n"/>
-      <c r="U16" s="5" t="n"/>
+      <c r="S16" s="6" t="n"/>
+      <c r="T16" s="5" t="n"/>
+      <c r="U16" s="6" t="n"/>
+      <c r="V16" s="5" t="n"/>
+      <c r="W16" s="7" t="n"/>
+      <c r="X16" s="7" t="n"/>
+      <c r="Y16" s="5" t="n"/>
     </row>
     <row r="17" ht="60" customHeight="1">
       <c r="A17" s="5" t="inlineStr">
@@ -1625,17 +1645,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="I17" s="5" t="inlineStr">
+      <c r="M17" s="5" t="inlineStr">
         <is>
           <t>Pointu</t>
         </is>
       </c>
-      <c r="J17" s="5" t="inlineStr">
+      <c r="N17" s="5" t="inlineStr">
         <is>
           <t>fil_infos_fil_info_262; rpn_rpn</t>
         </is>
       </c>
-      <c r="K17" s="5" t="inlineStr">
+      <c r="O17" s="5" t="inlineStr">
         <is>
           <t>1. Passage d'un règlement national-règlement intercours à un Code + RPN
 2. Séparation Code déontologie / Règlement professionnel
@@ -1644,20 +1664,20 @@
 5. Élaboration à quatre mains (profession + DACS)</t>
         </is>
       </c>
-      <c r="L17" s="5" t="inlineStr">
+      <c r="P17" s="5" t="inlineStr">
         <is>
           <t>La réforme 2021-2024 a remplacé l'ancien règlement national-règlement intercours par deux textes distincts : un Code de déontologie édicté par décret en Conseil d'État et un RPN approuvé par arrêté. Cette architecture donne une plus grande force juridique aux règles déontologiques et lie explicitement déontologie et discipline.</t>
         </is>
       </c>
-      <c r="M17" s="6" t="n"/>
-      <c r="N17" s="5" t="n"/>
-      <c r="O17" s="6" t="n"/>
-      <c r="P17" s="5" t="n"/>
       <c r="Q17" s="6" t="n"/>
       <c r="R17" s="5" t="n"/>
-      <c r="S17" s="7" t="n"/>
-      <c r="T17" s="7" t="n"/>
-      <c r="U17" s="5" t="n"/>
+      <c r="S17" s="6" t="n"/>
+      <c r="T17" s="5" t="n"/>
+      <c r="U17" s="6" t="n"/>
+      <c r="V17" s="5" t="n"/>
+      <c r="W17" s="7" t="n"/>
+      <c r="X17" s="7" t="n"/>
+      <c r="Y17" s="5" t="n"/>
     </row>
     <row r="18" ht="60" customHeight="1">
       <c r="A18" s="5" t="inlineStr">
@@ -1675,13 +1695,13 @@
           <t>Edge_Case</t>
         </is>
       </c>
-      <c r="I18" s="5" t="inlineStr">
+      <c r="M18" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="J18" s="5" t="inlineStr"/>
-      <c r="K18" s="5" t="inlineStr">
+      <c r="N18" s="5" t="inlineStr"/>
+      <c r="O18" s="5" t="inlineStr">
         <is>
           <t>1. Question hors périmètre de la Bible Notariale
 2. Concerne le parcours de formation
@@ -1689,20 +1709,20 @@
 4. Le chatbot devrait l'indiquer clairement</t>
         </is>
       </c>
-      <c r="L18" s="5" t="inlineStr">
+      <c r="P18" s="5" t="inlineStr">
         <is>
           <t>Cette question concerne le parcours de formation pour devenir notaire, ce qui est hors du périmètre des documents de la Bible Notariale qui se concentrent sur la déontologie, la CCN et les règles professionnelles pour les notaires en exercice. Le chatbot devrait indiquer qu'il ne dispose pas d'informations sur ce sujet.</t>
         </is>
       </c>
-      <c r="M18" s="6" t="n"/>
-      <c r="N18" s="5" t="n"/>
-      <c r="O18" s="6" t="n"/>
-      <c r="P18" s="5" t="n"/>
       <c r="Q18" s="6" t="n"/>
       <c r="R18" s="5" t="n"/>
-      <c r="S18" s="7" t="n"/>
-      <c r="T18" s="7" t="n"/>
-      <c r="U18" s="5" t="n"/>
+      <c r="S18" s="6" t="n"/>
+      <c r="T18" s="5" t="n"/>
+      <c r="U18" s="6" t="n"/>
+      <c r="V18" s="5" t="n"/>
+      <c r="W18" s="7" t="n"/>
+      <c r="X18" s="7" t="n"/>
+      <c r="Y18" s="5" t="n"/>
     </row>
     <row r="19" ht="60" customHeight="1">
       <c r="A19" s="5" t="inlineStr">
@@ -1720,13 +1740,13 @@
           <t>Edge_Case</t>
         </is>
       </c>
-      <c r="I19" s="5" t="inlineStr">
+      <c r="M19" s="5" t="inlineStr">
         <is>
           <t>Moyen</t>
         </is>
       </c>
-      <c r="J19" s="5" t="inlineStr"/>
-      <c r="K19" s="5" t="inlineStr">
+      <c r="N19" s="5" t="inlineStr"/>
+      <c r="O19" s="5" t="inlineStr">
         <is>
           <t>1. Question très large et historique
 2. Hors périmètre de la Bible Notariale
@@ -1734,20 +1754,20 @@
 4. Le chatbot devrait l'indiquer</t>
         </is>
       </c>
-      <c r="L19" s="5" t="inlineStr">
+      <c r="P19" s="5" t="inlineStr">
         <is>
           <t>Cette question sur l'histoire du notariat est trop large et hors du périmètre des documents de la Bible Notariale qui se concentrent sur l'actualité professionnelle, la déontologie actuelle et les règles en vigueur. Le chatbot devrait indiquer qu'il ne dispose pas d'informations historiques détaillées.</t>
         </is>
       </c>
-      <c r="M19" s="6" t="n"/>
-      <c r="N19" s="5" t="n"/>
-      <c r="O19" s="6" t="n"/>
-      <c r="P19" s="5" t="n"/>
       <c r="Q19" s="6" t="n"/>
       <c r="R19" s="5" t="n"/>
-      <c r="S19" s="7" t="n"/>
-      <c r="T19" s="7" t="n"/>
-      <c r="U19" s="5" t="n"/>
+      <c r="S19" s="6" t="n"/>
+      <c r="T19" s="5" t="n"/>
+      <c r="U19" s="6" t="n"/>
+      <c r="V19" s="5" t="n"/>
+      <c r="W19" s="7" t="n"/>
+      <c r="X19" s="7" t="n"/>
+      <c r="Y19" s="5" t="n"/>
     </row>
     <row r="20" ht="60" customHeight="1">
       <c r="A20" s="5" t="inlineStr">
@@ -1765,17 +1785,17 @@
           <t>Edge_Case</t>
         </is>
       </c>
-      <c r="I20" s="5" t="inlineStr">
+      <c r="M20" s="5" t="inlineStr">
         <is>
           <t>Pointu</t>
         </is>
       </c>
-      <c r="J20" s="5" t="inlineStr">
+      <c r="N20" s="5" t="inlineStr">
         <is>
           <t>fil_infos_fil_info_262; rpn_rpn; convention_collective_20241212_avenant_59_modif_art_29_5_participation_financiere_formation_pro_mis_; convention_collective_20241114_avenant_58_modif_art_15_6_et_29_3_3_mis_en_forme</t>
         </is>
       </c>
-      <c r="K20" s="5" t="inlineStr">
+      <c r="O20" s="5" t="inlineStr">
         <is>
           <t>1. Réforme déontologie : nouvelles exigences professionnelles
 2. CCN formation : mise en conformité avec obligations
@@ -1783,20 +1803,20 @@
 4. Période de transformation 2021-2024</t>
         </is>
       </c>
-      <c r="L20" s="5" t="inlineStr">
+      <c r="P20" s="5" t="inlineStr">
         <is>
           <t>La réforme de la déontologie (2021-2024) a établi de nouvelles exigences professionnelles, tandis que les modifications de la CCN sur la formation (avenants 58-59 en 2024) ont mis à jour les modalités de formation pour s'aligner sur ces nouvelles obligations. Ces évolutions parallèles illustrent la cohérence entre textes déontologiques et sociaux.</t>
         </is>
       </c>
-      <c r="M20" s="6" t="n"/>
-      <c r="N20" s="5" t="n"/>
-      <c r="O20" s="6" t="n"/>
-      <c r="P20" s="5" t="n"/>
       <c r="Q20" s="6" t="n"/>
       <c r="R20" s="5" t="n"/>
-      <c r="S20" s="7" t="n"/>
-      <c r="T20" s="7" t="n"/>
-      <c r="U20" s="5" t="n"/>
+      <c r="S20" s="6" t="n"/>
+      <c r="T20" s="5" t="n"/>
+      <c r="U20" s="6" t="n"/>
+      <c r="V20" s="5" t="n"/>
+      <c r="W20" s="7" t="n"/>
+      <c r="X20" s="7" t="n"/>
+      <c r="Y20" s="5" t="n"/>
     </row>
     <row r="21" ht="60" customHeight="1">
       <c r="A21" s="5" t="inlineStr">
@@ -1814,17 +1834,17 @@
           <t>Deontologie</t>
         </is>
       </c>
-      <c r="I21" s="5" t="inlineStr">
+      <c r="M21" s="5" t="inlineStr">
         <is>
           <t>Facile</t>
         </is>
       </c>
-      <c r="J21" s="5" t="inlineStr">
+      <c r="N21" s="5" t="inlineStr">
         <is>
           <t>rpn_rpn</t>
         </is>
       </c>
-      <c r="K21" s="5" t="inlineStr">
+      <c r="O21" s="5" t="inlineStr">
         <is>
           <t>1. Original de l'acte authentique
 2. Conservé par le notaire
@@ -1832,20 +1852,20 @@
 4. Seules des copies (expéditions) sont délivrées</t>
         </is>
       </c>
-      <c r="L21" s="5" t="inlineStr">
+      <c r="P21" s="5" t="inlineStr">
         <is>
           <t>La minute est l'original d'un acte authentique conservé par le notaire. C'est un document source qui ne peut quitter l'étude et dont seules des copies appelées expéditions sont délivrées aux parties.</t>
         </is>
       </c>
-      <c r="M21" s="6" t="n"/>
-      <c r="N21" s="5" t="n"/>
-      <c r="O21" s="6" t="n"/>
-      <c r="P21" s="5" t="n"/>
       <c r="Q21" s="6" t="n"/>
       <c r="R21" s="5" t="n"/>
-      <c r="S21" s="7" t="n"/>
-      <c r="T21" s="7" t="n"/>
-      <c r="U21" s="5" t="n"/>
+      <c r="S21" s="6" t="n"/>
+      <c r="T21" s="5" t="n"/>
+      <c r="U21" s="6" t="n"/>
+      <c r="V21" s="5" t="n"/>
+      <c r="W21" s="7" t="n"/>
+      <c r="X21" s="7" t="n"/>
+      <c r="Y21" s="5" t="n"/>
     </row>
   </sheetData>
   <dataValidations count="9">
@@ -1870,10 +1890,10 @@
     <dataValidation sqref="F2 F3 F4 F5 F6 F7 F8 F9 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" promptTitle="Source de document" prompt="Choisissez une source de document" type="list">
       <formula1>=Ref_SourcesDocument!$A$2:$A$9</formula1>
     </dataValidation>
-    <dataValidation sqref="G2 G3 G4 G5 G6 G7 G8 G9 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" promptTitle="Thématiques" prompt="Choisissez une ou plusieurs thématiques (séparées par des virgules)" type="list">
+    <dataValidation sqref="G2 G3 G4 G5 G6 G7 G8 G9 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21 H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 I2 I3 I4 I5 I6 I7 I8 I9 I10 I11 I12 I13 I14 I15 I16 I17 I18 I19 I20 I21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" promptTitle="Thématique" prompt="Choisissez une thématique" type="list">
       <formula1>=Ref_Thematiques!$A$2:$A$20</formula1>
     </dataValidation>
-    <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" promptTitle="Mots-clés" prompt="Choisissez un ou plusieurs mots-clés (séparés par des virgules)" type="list">
+    <dataValidation sqref="J2 J3 J4 J5 J6 J7 J8 J9 J10 J11 J12 J13 J14 J15 J16 J17 J18 J19 J20 J21 K2 K3 K4 K5 K6 K7 K8 K9 K10 K11 K12 K13 K14 K15 K16 K17 K18 K19 K20 K21 L2 L3 L4 L5 L6 L7 L8 L9 L10 L11 L12 L13 L14 L15 L16 L17 L18 L19 L20 L21" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" promptTitle="Mot-clé" prompt="Choisissez un mot-clé" type="list">
       <formula1>=Ref_MotsCles!$A$2:$A$46</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>